<commit_message>
refactor(core) modify core and generator
</commit_message>
<xml_diff>
--- a/数据库设计.xlsx
+++ b/数据库设计.xlsx
@@ -2451,9 +2451,9 @@
   <hyperlinks>
     <hyperlink ref="D3:E3" location="sys_user!A1" display="系统用户表"/>
     <hyperlink ref="D4:E4" location="sys_role!A1" display="系统角色表"/>
-    <hyperlink ref="D5:E5" location="sys_menu!A1" display="系统菜单表"/>
+    <hyperlink ref="D5:E5" location="sys_resource!A1" display="系统资源表"/>
     <hyperlink ref="D6:E6" location="sys_role_user!A1" display="系统角色用户关联表"/>
-    <hyperlink ref="D7:E7" location="sys_role_menu!A1" display="系统角色菜单关联表"/>
+    <hyperlink ref="D7:E7" location="sys_role_resource!A1" display="系统角色资源关联表"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>